<commit_message>
Reading user data from the excel sheet is implemented in the class ExcelDataFetch_Template
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginTestData.xlsx
+++ b/src/test/resources/testdata/LoginTestData.xlsx
@@ -3,24 +3,56 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eclipse workspaces\1. Automation Frameworks Tutorial Maven\EFTSwitchAutomation\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14200" windowHeight="4300"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="devTestLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginTest" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:N13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+  <si>
+    <t>USERNAME</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin1</t>
+  </si>
+  <si>
+    <t>useradmin</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>useadmin1</t>
+  </si>
+  <si>
+    <t>admina</t>
+  </si>
+  <si>
+    <t>useradmina</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,12 +368,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DataProvider is set on the excel sheet from the function internal array of the TestBase.class utils.ExcelUtil.java --> fuction to read the user data from excelsheet and provide the dataProvider to LoginTest.class
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginTestData.xlsx
+++ b/src/test/resources/testdata/LoginTestData.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14200" windowHeight="4300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14200" windowHeight="4300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="devTestLogin" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginTest" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginFunc" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <oleSize ref="A1:N13"/>
@@ -370,7 +370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Standardised the Home and UserRegistration pages in the POM pattern by removing the hardcording parts, Removed hard coding parts from the ExcelUtils and ExcelDataProvider classes, Added the user adding and deleting test cases in the class userregistrtionTest
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginTestData.xlsx
+++ b/src/test/resources/testdata/LoginTestData.xlsx
@@ -3,15 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eclipse workspaces\1. Automation Frameworks Tutorial Maven\EFTSwitchAutomation\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14200" windowHeight="4300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14020" windowHeight="5850" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="devTestLogin" sheetId="1" r:id="rId1"/>
     <sheet name="LoginFunc" sheetId="2" r:id="rId2"/>
+    <sheet name="userDetails" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:N13"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>USERNAME</t>
   </si>
@@ -51,16 +56,75 @@
   </si>
   <si>
     <t>useradmina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First  Name </t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email ID</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>User Name</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>sujith@gmail.com</t>
+  </si>
+  <si>
+    <t>Login user</t>
+  </si>
+  <si>
+    <t>Login password</t>
+  </si>
+  <si>
+    <t>jith</t>
+  </si>
+  <si>
+    <t>userjith</t>
+  </si>
+  <si>
+    <t>jith1</t>
+  </si>
+  <si>
+    <t>Sujith123</t>
+  </si>
+  <si>
+    <t>Sujith456</t>
+  </si>
+  <si>
+    <t>css</t>
+  </si>
+  <si>
+    <t>cs123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,13 +147,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -368,7 +435,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -384,7 +451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -392,7 +459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -400,7 +467,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -408,7 +475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -416,7 +483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -424,7 +491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -432,7 +499,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -440,7 +507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -448,7 +515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -456,7 +523,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -466,7 +532,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -515,4 +581,124 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2">
+        <v>123456</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3">
+        <v>1234566</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
the last row of the excel sheet was not being read. fixed the row boundary length in the array and in the for loop
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginTestData.xlsx
+++ b/src/test/resources/testdata/LoginTestData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\eclipse workspaces\1. Automation Frameworks Tutorial Maven\EFTSwitchAutomation\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14020" windowHeight="5850" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="4140" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="devTestLogin" sheetId="1" r:id="rId1"/>
@@ -17,6 +12,7 @@
     <sheet name="userDetails" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:I12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -533,7 +529,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -585,10 +581,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,9 +687,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C4" s="1"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>

</xml_diff>

<commit_message>
TestNG functionalities integration: -screenshot - listener -default reporting - listener,xml -custom reporting - xml,pom(dependency and plugins) -retry analyzer - listener,xml -retry anlayzer - @Test
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginTestData.xlsx
+++ b/src/test/resources/testdata/LoginTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="4140" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="4140" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="devTestLogin" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="userDetails" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I12"/>
+  <oleSize ref="A1:M12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -583,7 +583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
excel data sheet upddated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginTestData.xlsx
+++ b/src/test/resources/testdata/LoginTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="4140" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="4140" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="devTestLogin" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,10 @@
     <sheet name="sysConfDetails" sheetId="4" r:id="rId4"/>
     <sheet name="RCDetails" sheetId="5" r:id="rId5"/>
     <sheet name="DGDetails" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet4" sheetId="7" r:id="rId7"/>
+    <sheet name="CGDetails" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId8"/>
+    <sheet name="BINDetails" sheetId="8" r:id="rId9"/>
+    <sheet name="RouteDetails" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="154">
   <si>
     <t>USERNAME</t>
   </si>
@@ -234,13 +237,271 @@
   </si>
   <si>
     <t>AtmDg</t>
+  </si>
+  <si>
+    <t>paramName1</t>
+  </si>
+  <si>
+    <t>tr1</t>
+  </si>
+  <si>
+    <t>td1</t>
+  </si>
+  <si>
+    <t>paramName2</t>
+  </si>
+  <si>
+    <t>tr2</t>
+  </si>
+  <si>
+    <t>td2</t>
+  </si>
+  <si>
+    <t>bin_tr</t>
+  </si>
+  <si>
+    <t>bin_td</t>
+  </si>
+  <si>
+    <t>bin_td_del-btn</t>
+  </si>
+  <si>
+    <t>cardGrp_tr</t>
+  </si>
+  <si>
+    <t>cardGrp_td</t>
+  </si>
+  <si>
+    <t>cardGrp_td_Viewbtn</t>
+  </si>
+  <si>
+    <t>bin</t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>Edit btn</t>
+  </si>
+  <si>
+    <t>Del btn</t>
+  </si>
+  <si>
+    <t>Dsescri</t>
+  </si>
+  <si>
+    <t>BIN len</t>
+  </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>EVRTEC</t>
+  </si>
+  <si>
+    <t>MDS</t>
+  </si>
+  <si>
+    <t>NGO</t>
+  </si>
+  <si>
+    <t>VISA</t>
+  </si>
+  <si>
+    <t>bin_td_edit_btn</t>
+  </si>
+  <si>
+    <t>cardGrp_td_Editbtn</t>
+  </si>
+  <si>
+    <t>tdEditbtnCG</t>
+  </si>
+  <si>
+    <t>tdEditbtnBIN</t>
+  </si>
+  <si>
+    <t>tdViewbtnCG</t>
+  </si>
+  <si>
+    <t>tdDeletebtnBIN</t>
+  </si>
+  <si>
+    <t>CG_value1</t>
+  </si>
+  <si>
+    <t>CG_value2</t>
+  </si>
+  <si>
+    <t>CG_value3</t>
+  </si>
+  <si>
+    <t>CG_value4</t>
+  </si>
+  <si>
+    <t>CG_value5</t>
+  </si>
+  <si>
+    <t>RC_option_ATMRC</t>
+  </si>
+  <si>
+    <t>RC_option_MdsRC</t>
+  </si>
+  <si>
+    <t>RC_option_NaiguataRC</t>
+  </si>
+  <si>
+    <t>RC_option_VisaRC</t>
+  </si>
+  <si>
+    <t>bin_1</t>
+  </si>
+  <si>
+    <t>bin_2</t>
+  </si>
+  <si>
+    <t>bin_3</t>
+  </si>
+  <si>
+    <t>bin_4</t>
+  </si>
+  <si>
+    <t>bin_5</t>
+  </si>
+  <si>
+    <t>RC_option_EvertecCredRC</t>
+  </si>
+  <si>
+    <t>MDS-BIN-Number1</t>
+  </si>
+  <si>
+    <t>MDS-BIN-Number3</t>
+  </si>
+  <si>
+    <t>MDS-BIN-Number5</t>
+  </si>
+  <si>
+    <t>MDS-BIN-Number7</t>
+  </si>
+  <si>
+    <t>MDS-BIN-Number8</t>
+  </si>
+  <si>
+    <t>MDS-BIN-Number2</t>
+  </si>
+  <si>
+    <t>MDS-BIN-Number4</t>
+  </si>
+  <si>
+    <t>MDS-BIN-Number6</t>
+  </si>
+  <si>
+    <t>MDSCR-BIN-Number1</t>
+  </si>
+  <si>
+    <t>CMS-BIN-Number1</t>
+  </si>
+  <si>
+    <t>CMS-BIN-Number2</t>
+  </si>
+  <si>
+    <t>CMS-BIN-Number3</t>
+  </si>
+  <si>
+    <t>CMS-BIN-Number4</t>
+  </si>
+  <si>
+    <t>CMS-BIN-Number5</t>
+  </si>
+  <si>
+    <t>CMS-BIN-Number6</t>
+  </si>
+  <si>
+    <t>CMS-BIN-Number7</t>
+  </si>
+  <si>
+    <t>CMS-BIN-Number8</t>
+  </si>
+  <si>
+    <t>NGO-BIN-Number1</t>
+  </si>
+  <si>
+    <t>NGO-BIN-Number2</t>
+  </si>
+  <si>
+    <t>NGO-BIN-Number3</t>
+  </si>
+  <si>
+    <t>NGO-BIN-Number4</t>
+  </si>
+  <si>
+    <t>NGO-BIN-Number5</t>
+  </si>
+  <si>
+    <t>NGO-BIN-Number6</t>
+  </si>
+  <si>
+    <t>NGO-BIN-Number7</t>
+  </si>
+  <si>
+    <t>NGO-BIN-Number8</t>
+  </si>
+  <si>
+    <t>NGO-BIN-Number9</t>
+  </si>
+  <si>
+    <t>NGO-BIN-Number10</t>
+  </si>
+  <si>
+    <t>Visa-BIN-Number1</t>
+  </si>
+  <si>
+    <t>Visa-BIN-Number2</t>
+  </si>
+  <si>
+    <t>Visa-BIN-Number3</t>
+  </si>
+  <si>
+    <t>Visa-BIN-Number4</t>
+  </si>
+  <si>
+    <t>Visa-BIN-Number5</t>
+  </si>
+  <si>
+    <t>Visa-BIN-Number6</t>
+  </si>
+  <si>
+    <t>Visa-BIN-Number7</t>
+  </si>
+  <si>
+    <t>Visa-BIN-Number8</t>
+  </si>
+  <si>
+    <t>bin_descr</t>
+  </si>
+  <si>
+    <t>pan_len</t>
+  </si>
+  <si>
+    <t>bin_len</t>
+  </si>
+  <si>
+    <t>route_tr</t>
+  </si>
+  <si>
+    <t>route_td</t>
+  </si>
+  <si>
+    <t>route_tdbtn</t>
+  </si>
+  <si>
+    <t>tdEditbtnRoute</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,16 +517,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF5F5F5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -273,17 +546,38 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -658,6 +952,56 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
@@ -1108,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1197,14 +1541,1591 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H3"/>
+      <selection activeCell="B2" sqref="B2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" t="s">
+        <v>76</v>
+      </c>
+      <c r="J2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J3" t="s">
+        <v>92</v>
+      </c>
+      <c r="K3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>91</v>
+      </c>
+      <c r="I5" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J6" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" t="s">
+        <v>86</v>
+      </c>
+      <c r="S1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T1" t="s">
+        <v>85</v>
+      </c>
+      <c r="U1" t="s">
+        <v>81</v>
+      </c>
+      <c r="V1" t="s">
+        <v>82</v>
+      </c>
+      <c r="W1" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>123123</v>
+      </c>
+      <c r="I2" s="3">
+        <v>501878</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>485046</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>588891</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>58990</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>311112</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>510874</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>589524</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>414764</v>
+      </c>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>543210</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>518309</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>601288</v>
+      </c>
+      <c r="AG4" s="3">
+        <v>418021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>568767</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>531127</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>602000</v>
+      </c>
+      <c r="AG5" s="3">
+        <v>422123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>585948</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>531260</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>603061</v>
+      </c>
+      <c r="AG6" s="3">
+        <v>499929</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>788965</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>559843</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>603122</v>
+      </c>
+      <c r="AG7" s="3">
+        <v>526749</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>867580</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>621984</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>603208</v>
+      </c>
+      <c r="AG8" s="3">
+        <v>541333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4">
+        <v>898965</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>5267445</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>603256</v>
+      </c>
+      <c r="AG9" s="3">
+        <v>552311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="Y10" s="3">
+        <v>627609</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="Y11" s="3">
+        <v>639489</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.77734375" customWidth="1"/>
+    <col min="17" max="17" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="3.21875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="6.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E2" s="6">
+        <v>123123</v>
+      </c>
+      <c r="F2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="5">
+        <v>16</v>
+      </c>
+      <c r="H2" s="5">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="6">
+        <v>311112</v>
+      </c>
+      <c r="F3" t="s">
+        <v>122</v>
+      </c>
+      <c r="G3" s="5">
+        <v>16</v>
+      </c>
+      <c r="H3" s="5">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="6">
+        <v>543210</v>
+      </c>
+      <c r="F4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="5">
+        <v>16</v>
+      </c>
+      <c r="H4" s="5">
+        <v>6</v>
+      </c>
+      <c r="I4" t="s">
+        <v>102</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="6">
+        <v>568767</v>
+      </c>
+      <c r="F5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" s="5">
+        <v>16</v>
+      </c>
+      <c r="H5" s="5">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>102</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="6">
+        <v>585948</v>
+      </c>
+      <c r="F6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="5">
+        <v>16</v>
+      </c>
+      <c r="H6" s="5">
+        <v>6</v>
+      </c>
+      <c r="I6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="6">
+        <v>788965</v>
+      </c>
+      <c r="F7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" s="5">
+        <v>16</v>
+      </c>
+      <c r="H7" s="5">
+        <v>6</v>
+      </c>
+      <c r="I7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="6">
+        <v>867580</v>
+      </c>
+      <c r="F8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" s="5">
+        <v>16</v>
+      </c>
+      <c r="H8" s="5">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E9" s="6">
+        <v>898965</v>
+      </c>
+      <c r="F9" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="5">
+        <v>16</v>
+      </c>
+      <c r="H9" s="5">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="6">
+        <v>485046</v>
+      </c>
+      <c r="F10" t="s">
+        <v>112</v>
+      </c>
+      <c r="G10" s="5">
+        <v>16</v>
+      </c>
+      <c r="H10" s="5">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="6">
+        <v>510874</v>
+      </c>
+      <c r="F11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="5">
+        <v>16</v>
+      </c>
+      <c r="H11" s="5">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="6">
+        <v>518309</v>
+      </c>
+      <c r="F12" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="5">
+        <v>16</v>
+      </c>
+      <c r="H12" s="5">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="6">
+        <v>531127</v>
+      </c>
+      <c r="F13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" s="5">
+        <v>16</v>
+      </c>
+      <c r="H13" s="5">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E14" s="6">
+        <v>531260</v>
+      </c>
+      <c r="F14" t="s">
+        <v>114</v>
+      </c>
+      <c r="G14" s="5">
+        <v>16</v>
+      </c>
+      <c r="H14" s="5">
+        <v>6</v>
+      </c>
+      <c r="I14" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="6">
+        <v>559843</v>
+      </c>
+      <c r="F15" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="5">
+        <v>16</v>
+      </c>
+      <c r="H15" s="5">
+        <v>6</v>
+      </c>
+      <c r="I15" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="6">
+        <v>621984</v>
+      </c>
+      <c r="F16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="5">
+        <v>16</v>
+      </c>
+      <c r="H16" s="5">
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="6">
+        <v>5267445</v>
+      </c>
+      <c r="F17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" s="5">
+        <v>16</v>
+      </c>
+      <c r="H17" s="5">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="6">
+        <v>501878</v>
+      </c>
+      <c r="F18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" s="5">
+        <v>16</v>
+      </c>
+      <c r="H18" s="5">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="6">
+        <v>588891</v>
+      </c>
+      <c r="F19" t="s">
+        <v>129</v>
+      </c>
+      <c r="G19" s="5">
+        <v>16</v>
+      </c>
+      <c r="H19" s="5">
+        <v>6</v>
+      </c>
+      <c r="I19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="6">
+        <v>589524</v>
+      </c>
+      <c r="F20" t="s">
+        <v>130</v>
+      </c>
+      <c r="G20" s="5">
+        <v>16</v>
+      </c>
+      <c r="H20" s="5">
+        <v>6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="6">
+        <v>601288</v>
+      </c>
+      <c r="F21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G21" s="5">
+        <v>16</v>
+      </c>
+      <c r="H21" s="5">
+        <v>6</v>
+      </c>
+      <c r="I21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" t="s">
+        <v>78</v>
+      </c>
+      <c r="D22" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="6">
+        <v>602000</v>
+      </c>
+      <c r="F22" t="s">
+        <v>132</v>
+      </c>
+      <c r="G22" s="5">
+        <v>16</v>
+      </c>
+      <c r="H22" s="5">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" s="6">
+        <v>603061</v>
+      </c>
+      <c r="F23" t="s">
+        <v>133</v>
+      </c>
+      <c r="G23" s="5">
+        <v>16</v>
+      </c>
+      <c r="H23" s="5">
+        <v>6</v>
+      </c>
+      <c r="I23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" s="6">
+        <v>603122</v>
+      </c>
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" s="5">
+        <v>16</v>
+      </c>
+      <c r="H24" s="5">
+        <v>6</v>
+      </c>
+      <c r="I24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>100</v>
+      </c>
+      <c r="B25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="6">
+        <v>603208</v>
+      </c>
+      <c r="F25" t="s">
+        <v>135</v>
+      </c>
+      <c r="G25" s="5">
+        <v>16</v>
+      </c>
+      <c r="H25" s="5">
+        <v>6</v>
+      </c>
+      <c r="I25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="6">
+        <v>603256</v>
+      </c>
+      <c r="F26" t="s">
+        <v>136</v>
+      </c>
+      <c r="G26" s="5">
+        <v>16</v>
+      </c>
+      <c r="H26" s="5">
+        <v>6</v>
+      </c>
+      <c r="I26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s">
+        <v>79</v>
+      </c>
+      <c r="E27" s="6">
+        <v>627609</v>
+      </c>
+      <c r="F27" t="s">
+        <v>137</v>
+      </c>
+      <c r="G27" s="5">
+        <v>16</v>
+      </c>
+      <c r="H27" s="5">
+        <v>6</v>
+      </c>
+      <c r="I27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="6">
+        <v>639489</v>
+      </c>
+      <c r="F28" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="5">
+        <v>16</v>
+      </c>
+      <c r="H28" s="5">
+        <v>6</v>
+      </c>
+      <c r="I28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="6">
+        <v>58990</v>
+      </c>
+      <c r="F29" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29" s="5">
+        <v>16</v>
+      </c>
+      <c r="H29" s="5">
+        <v>6</v>
+      </c>
+      <c r="I29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>101</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="6">
+        <v>414764</v>
+      </c>
+      <c r="F30" t="s">
+        <v>140</v>
+      </c>
+      <c r="G30" s="5">
+        <v>16</v>
+      </c>
+      <c r="H30" s="5">
+        <v>6</v>
+      </c>
+      <c r="I30" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="6">
+        <v>418021</v>
+      </c>
+      <c r="F31" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="5">
+        <v>16</v>
+      </c>
+      <c r="H31" s="5">
+        <v>6</v>
+      </c>
+      <c r="I31" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>101</v>
+      </c>
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" s="6">
+        <v>422123</v>
+      </c>
+      <c r="F32" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="5">
+        <v>16</v>
+      </c>
+      <c r="H32" s="5">
+        <v>6</v>
+      </c>
+      <c r="I32" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" t="s">
+        <v>77</v>
+      </c>
+      <c r="C33" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" s="6">
+        <v>499929</v>
+      </c>
+      <c r="F33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33" s="5">
+        <v>16</v>
+      </c>
+      <c r="H33" s="5">
+        <v>6</v>
+      </c>
+      <c r="I33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>101</v>
+      </c>
+      <c r="B34" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" t="s">
+        <v>78</v>
+      </c>
+      <c r="D34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="6">
+        <v>526749</v>
+      </c>
+      <c r="F34" t="s">
+        <v>144</v>
+      </c>
+      <c r="G34" s="5">
+        <v>16</v>
+      </c>
+      <c r="H34" s="5">
+        <v>6</v>
+      </c>
+      <c r="I34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" t="s">
+        <v>78</v>
+      </c>
+      <c r="D35" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" s="6">
+        <v>541333</v>
+      </c>
+      <c r="F35" t="s">
+        <v>145</v>
+      </c>
+      <c r="G35" s="5">
+        <v>16</v>
+      </c>
+      <c r="H35" s="5">
+        <v>6</v>
+      </c>
+      <c r="I35" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36" s="6">
+        <v>552311</v>
+      </c>
+      <c r="F36" t="s">
+        <v>146</v>
+      </c>
+      <c r="G36" s="5">
+        <v>16</v>
+      </c>
+      <c r="H36" s="5">
+        <v>6</v>
+      </c>
+      <c r="I36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
0200 and 0420 messges sending to the respective interfaces - fuction testing module implemented
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginTestData.xlsx
+++ b/src/test/resources/testdata/LoginTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="4140" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="4140" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="devTestLogin" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="RCDetails" sheetId="5" r:id="rId5"/>
     <sheet name="DGDetails" sheetId="6" r:id="rId6"/>
     <sheet name="CGDetails" sheetId="7" r:id="rId7"/>
-    <sheet name="BINDetails" sheetId="8" r:id="rId8"/>
-    <sheet name="RouteDetails" sheetId="10" r:id="rId9"/>
-    <sheet name="AlphaNodeDetails" sheetId="11" r:id="rId10"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId8"/>
+    <sheet name="BINDetails" sheetId="8" r:id="rId9"/>
+    <sheet name="RouteDetails" sheetId="10" r:id="rId10"/>
+    <sheet name="AlphaNodeDetails" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="159">
   <si>
     <t>USERNAME</t>
   </si>
@@ -210,9 +210,6 @@
     <t>ATMRC</t>
   </si>
   <si>
-    <t>EvertecCred</t>
-  </si>
-  <si>
     <t>NaiguataRC</t>
   </si>
   <si>
@@ -493,13 +490,34 @@
   </si>
   <si>
     <t>alphaNode_port_SwitchAlpha</t>
+  </si>
+  <si>
+    <t>CMSCardGroup</t>
+  </si>
+  <si>
+    <t>MasterCard</t>
+  </si>
+  <si>
+    <t>MasterCardCR</t>
+  </si>
+  <si>
+    <t>Naiguata</t>
+  </si>
+  <si>
+    <t>Visa</t>
+  </si>
+  <si>
+    <t>VisaRC</t>
+  </si>
+  <si>
+    <t>EvertecCredRC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +538,13 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -543,7 +568,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -552,6 +577,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -928,10 +954,60 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -944,34 +1020,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" t="s">
         <v>145</v>
-      </c>
-      <c r="B1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -985,7 +1061,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1157,7 +1233,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1336,15 +1412,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.21875" bestFit="1" customWidth="1"/>
@@ -1381,7 +1457,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>158</v>
       </c>
       <c r="B3" t="s">
         <v>54</v>
@@ -1395,7 +1471,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" t="s">
         <v>54</v>
@@ -1409,7 +1485,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
         <v>54</v>
@@ -1418,6 +1494,20 @@
         <v>55</v>
       </c>
       <c r="D5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1457,58 +1547,58 @@
         <v>52</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" t="s">
         <v>62</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>63</v>
       </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
       <c r="E2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
         <v>62</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>63</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>64</v>
-      </c>
-      <c r="E3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>63</v>
       </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1519,10 +1609,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1539,214 +1629,244 @@
     <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
         <v>70</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" t="s">
         <v>86</v>
       </c>
-      <c r="E1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2">
+        <v>123456</v>
+      </c>
+      <c r="F2" t="s">
         <v>73</v>
       </c>
-      <c r="H1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="J1" t="s">
-        <v>84</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="O2" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3">
+        <v>123457</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" t="s">
+        <v>93</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="O3" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4">
+        <v>123458</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
         <v>74</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" t="s">
         <v>75</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J4" t="s">
         <v>82</v>
       </c>
-      <c r="I2" t="s">
-        <v>76</v>
-      </c>
-      <c r="J2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="K4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="O4" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5">
+        <v>123459</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
         <v>74</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" t="s">
         <v>75</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J5" t="s">
         <v>82</v>
       </c>
-      <c r="I3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J3" t="s">
-        <v>83</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="K5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="M5" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="B4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="O5" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="F4" t="s">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6">
+        <v>123460</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
         <v>74</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" t="s">
         <v>75</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J6" t="s">
         <v>82</v>
       </c>
-      <c r="I4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J4" t="s">
-        <v>83</v>
-      </c>
-      <c r="K4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="K6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M6" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="O6" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="F5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" t="s">
-        <v>75</v>
-      </c>
-      <c r="H5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" t="s">
-        <v>75</v>
-      </c>
-      <c r="H6" t="s">
-        <v>82</v>
-      </c>
-      <c r="I6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J6" t="s">
-        <v>83</v>
-      </c>
-      <c r="K6" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1757,10 +1877,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1806,52 +1940,52 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="F1" t="s">
-        <v>138</v>
-      </c>
-      <c r="G1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H1" t="s">
-        <v>140</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" s="5">
         <v>123123</v>
       </c>
       <c r="F2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G2" s="4">
         <v>16</v>
@@ -1860,28 +1994,28 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="5">
         <v>311112</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="4">
         <v>16</v>
@@ -1890,28 +2024,28 @@
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E4" s="5">
         <v>543210</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G4" s="4">
         <v>16</v>
@@ -1920,28 +2054,28 @@
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E5" s="5">
         <v>568767</v>
       </c>
       <c r="F5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G5" s="4">
         <v>16</v>
@@ -1950,28 +2084,28 @@
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="5">
         <v>585948</v>
       </c>
       <c r="F6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G6" s="4">
         <v>16</v>
@@ -1980,28 +2114,28 @@
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="5">
         <v>788965</v>
       </c>
       <c r="F7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G7" s="4">
         <v>16</v>
@@ -2010,28 +2144,28 @@
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="5">
         <v>867580</v>
       </c>
       <c r="F8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G8" s="4">
         <v>16</v>
@@ -2040,27 +2174,27 @@
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" s="5">
         <v>898965</v>
       </c>
       <c r="F9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G9" s="4">
         <v>16</v>
@@ -2069,27 +2203,27 @@
         <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E10" s="5">
         <v>485046</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G10" s="4">
         <v>16</v>
@@ -2098,27 +2232,27 @@
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E11" s="5">
         <v>510874</v>
       </c>
       <c r="F11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G11" s="4">
         <v>16</v>
@@ -2127,27 +2261,27 @@
         <v>6</v>
       </c>
       <c r="I11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" s="5">
         <v>518309</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G12" s="4">
         <v>16</v>
@@ -2156,27 +2290,27 @@
         <v>6</v>
       </c>
       <c r="I12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="5">
         <v>531127</v>
       </c>
       <c r="F13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G13" s="4">
         <v>16</v>
@@ -2185,27 +2319,27 @@
         <v>6</v>
       </c>
       <c r="I13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E14" s="5">
         <v>531260</v>
       </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G14" s="4">
         <v>16</v>
@@ -2214,27 +2348,27 @@
         <v>6</v>
       </c>
       <c r="I14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E15" s="5">
         <v>559843</v>
       </c>
       <c r="F15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G15" s="4">
         <v>16</v>
@@ -2243,27 +2377,27 @@
         <v>6</v>
       </c>
       <c r="I15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="5">
         <v>621984</v>
       </c>
       <c r="F16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G16" s="4">
         <v>16</v>
@@ -2272,27 +2406,27 @@
         <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>153</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E17" s="5">
         <v>5267445</v>
       </c>
       <c r="F17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G17" s="4">
         <v>16</v>
@@ -2301,27 +2435,27 @@
         <v>6</v>
       </c>
       <c r="I17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>90</v>
+        <v>154</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E18" s="5">
         <v>501878</v>
       </c>
       <c r="F18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G18" s="4">
         <v>16</v>
@@ -2330,27 +2464,27 @@
         <v>6</v>
       </c>
       <c r="I18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E19" s="5">
         <v>588891</v>
       </c>
       <c r="F19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G19" s="4">
         <v>16</v>
@@ -2359,27 +2493,27 @@
         <v>6</v>
       </c>
       <c r="I19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E20" s="5">
         <v>589524</v>
       </c>
       <c r="F20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G20" s="4">
         <v>16</v>
@@ -2388,27 +2522,27 @@
         <v>6</v>
       </c>
       <c r="I20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" s="5">
         <v>601288</v>
       </c>
       <c r="F21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G21" s="4">
         <v>16</v>
@@ -2417,27 +2551,27 @@
         <v>6</v>
       </c>
       <c r="I21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E22" s="5">
         <v>602000</v>
       </c>
       <c r="F22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G22" s="4">
         <v>16</v>
@@ -2446,27 +2580,27 @@
         <v>6</v>
       </c>
       <c r="I22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E23" s="5">
         <v>603061</v>
       </c>
       <c r="F23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G23" s="4">
         <v>16</v>
@@ -2475,27 +2609,27 @@
         <v>6</v>
       </c>
       <c r="I23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E24" s="5">
         <v>603122</v>
       </c>
       <c r="F24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G24" s="4">
         <v>16</v>
@@ -2504,27 +2638,27 @@
         <v>6</v>
       </c>
       <c r="I24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E25" s="5">
         <v>603208</v>
       </c>
       <c r="F25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G25" s="4">
         <v>16</v>
@@ -2533,27 +2667,27 @@
         <v>6</v>
       </c>
       <c r="I25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E26" s="5">
         <v>603256</v>
       </c>
       <c r="F26" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G26" s="4">
         <v>16</v>
@@ -2562,27 +2696,27 @@
         <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E27" s="5">
         <v>627609</v>
       </c>
       <c r="F27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G27" s="4">
         <v>16</v>
@@ -2591,27 +2725,27 @@
         <v>6</v>
       </c>
       <c r="I27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>155</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E28" s="5">
         <v>639489</v>
       </c>
       <c r="F28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G28" s="4">
         <v>16</v>
@@ -2620,27 +2754,27 @@
         <v>6</v>
       </c>
       <c r="I28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E29" s="5">
         <v>58990</v>
       </c>
       <c r="F29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G29" s="4">
         <v>16</v>
@@ -2649,27 +2783,27 @@
         <v>6</v>
       </c>
       <c r="I29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E30" s="5">
         <v>414764</v>
       </c>
       <c r="F30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G30" s="4">
         <v>16</v>
@@ -2678,27 +2812,27 @@
         <v>6</v>
       </c>
       <c r="I30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" s="5">
         <v>418021</v>
       </c>
       <c r="F31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G31" s="4">
         <v>16</v>
@@ -2707,27 +2841,27 @@
         <v>6</v>
       </c>
       <c r="I31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E32" s="5">
         <v>422123</v>
       </c>
       <c r="F32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G32" s="4">
         <v>16</v>
@@ -2736,27 +2870,27 @@
         <v>6</v>
       </c>
       <c r="I32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="B33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E33" s="5">
         <v>499929</v>
       </c>
       <c r="F33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G33" s="4">
         <v>16</v>
@@ -2765,27 +2899,27 @@
         <v>6</v>
       </c>
       <c r="I33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E34" s="5">
         <v>526749</v>
       </c>
       <c r="F34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G34" s="4">
         <v>16</v>
@@ -2794,27 +2928,27 @@
         <v>6</v>
       </c>
       <c r="I34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="B35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E35" s="5">
         <v>541333</v>
       </c>
       <c r="F35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G35" s="4">
         <v>16</v>
@@ -2823,27 +2957,27 @@
         <v>6</v>
       </c>
       <c r="I35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E36" s="5">
         <v>552311</v>
       </c>
       <c r="F36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G36" s="4">
         <v>16</v>
@@ -2852,57 +2986,7 @@
         <v>6</v>
       </c>
       <c r="I36" t="s">
-        <v>96</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" t="s">
-        <v>143</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
standardised the modules nodeApp, interchanges, routes. function-test-suites differenciated with regression-suite and created two function suites for command-fuction testing and positive-fuction-testing-scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/LoginTestData.xlsx
+++ b/src/test/resources/testdata/LoginTestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="4140" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12840" windowHeight="4140" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="devTestLogin" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="170">
   <si>
     <t>USERNAME</t>
   </si>
@@ -511,6 +511,39 @@
   </si>
   <si>
     <t>EvertecCredRC</t>
+  </si>
+  <si>
+    <t>option_routes_dg3</t>
+  </si>
+  <si>
+    <t>option_routes_dg</t>
+  </si>
+  <si>
+    <t>option_routes_cg2</t>
+  </si>
+  <si>
+    <t>option_routes_cg</t>
+  </si>
+  <si>
+    <t>option_routes_omega1</t>
+  </si>
+  <si>
+    <t>option_routes_omega</t>
+  </si>
+  <si>
+    <t>option_routes_rc</t>
+  </si>
+  <si>
+    <t>option_routes_rc3</t>
+  </si>
+  <si>
+    <t>option_routes_cg4</t>
+  </si>
+  <si>
+    <t>option_routes_omega2</t>
+  </si>
+  <si>
+    <t>option_routes_rc1</t>
   </si>
 </sst>
 </file>
@@ -954,10 +987,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -966,9 +999,13 @@
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -981,10 +1018,22 @@
       <c r="D1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G1" t="s">
+        <v>164</v>
+      </c>
+      <c r="H1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>140</v>
@@ -994,6 +1043,44 @@
       </c>
       <c r="D2" t="s">
         <v>142</v>
+      </c>
+      <c r="E2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F3" t="s">
+        <v>161</v>
+      </c>
+      <c r="G3" t="s">
+        <v>163</v>
+      </c>
+      <c r="H3" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1414,7 +1501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1612,7 +1699,7 @@
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1624,9 +1711,13 @@
     <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.21875" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -1658,9 +1749,18 @@
         <v>86</v>
       </c>
       <c r="J1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="K1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L1" t="s">
+        <v>138</v>
+      </c>
+      <c r="M1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N1" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1692,18 +1792,22 @@
       <c r="I2" t="s">
         <v>75</v>
       </c>
-      <c r="J2" t="s">
-        <v>82</v>
+      <c r="J2">
+        <v>123456</v>
       </c>
       <c r="K2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L2" s="4">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4">
+        <v>6</v>
+      </c>
+      <c r="N2" t="s">
         <v>92</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>96</v>
-      </c>
+      <c r="O2" s="6"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1733,18 +1837,22 @@
       <c r="I3" t="s">
         <v>75</v>
       </c>
-      <c r="J3" t="s">
-        <v>82</v>
+      <c r="J3">
+        <v>123457</v>
       </c>
       <c r="K3" t="s">
+        <v>102</v>
+      </c>
+      <c r="L3" s="4">
+        <v>16</v>
+      </c>
+      <c r="M3" s="4">
+        <v>6</v>
+      </c>
+      <c r="N3" t="s">
         <v>93</v>
       </c>
-      <c r="M3" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>97</v>
-      </c>
+      <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1774,18 +1882,22 @@
       <c r="I4" t="s">
         <v>75</v>
       </c>
-      <c r="J4" t="s">
-        <v>82</v>
+      <c r="J4">
+        <v>123458</v>
       </c>
       <c r="K4" t="s">
+        <v>110</v>
+      </c>
+      <c r="L4" s="4">
+        <v>16</v>
+      </c>
+      <c r="M4" s="4">
+        <v>6</v>
+      </c>
+      <c r="N4" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>98</v>
-      </c>
+      <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -1815,18 +1927,22 @@
       <c r="I5" t="s">
         <v>75</v>
       </c>
-      <c r="J5" t="s">
-        <v>82</v>
+      <c r="J5">
+        <v>123459</v>
       </c>
       <c r="K5" t="s">
+        <v>119</v>
+      </c>
+      <c r="L5" s="4">
+        <v>16</v>
+      </c>
+      <c r="M5" s="4">
+        <v>6</v>
+      </c>
+      <c r="N5" t="s">
         <v>94</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>99</v>
-      </c>
+      <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -1856,18 +1972,22 @@
       <c r="I6" t="s">
         <v>75</v>
       </c>
-      <c r="J6" t="s">
-        <v>82</v>
+      <c r="J6">
+        <v>123460</v>
       </c>
       <c r="K6" t="s">
+        <v>129</v>
+      </c>
+      <c r="L6" s="4">
+        <v>16</v>
+      </c>
+      <c r="M6" s="4">
+        <v>6</v>
+      </c>
+      <c r="N6" t="s">
         <v>95</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>100</v>
-      </c>
+      <c r="O6" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1877,14 +1997,255 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:O5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2">
+        <v>123456</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K2" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3">
+        <v>123457</v>
+      </c>
+      <c r="F3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K3" t="s">
+        <v>93</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4">
+        <v>123458</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K4" t="s">
+        <v>101</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5">
+        <v>123459</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K5" t="s">
+        <v>94</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E6">
+        <v>123460</v>
+      </c>
+      <c r="F6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1893,8 +2254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I29" sqref="E29:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>